<commit_message>
Adding files to sourcepath
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ojas Gupta\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ojas Gupta\Desktop\JAVA\placementQuestions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{554761E1-3A03-4BD6-AAD7-E2B771F0BE12}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA319078-3981-4D5D-BF8C-44D6E56BFC37}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1352" uniqueCount="465">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1352" uniqueCount="466">
   <si>
     <t>Topic:</t>
   </si>
@@ -1426,6 +1426,9 @@
   </si>
   <si>
     <t>Questions by Ojas Gupta:</t>
+  </si>
+  <si>
+    <t>YES</t>
   </si>
 </sst>
 </file>
@@ -1858,7 +1861,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -1902,7 +1905,7 @@
         <v>5</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>3</v>
+        <v>465</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="21">
@@ -1913,7 +1916,7 @@
         <v>6</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>3</v>
+        <v>465</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="21">

</xml_diff>